<commit_message>
Update to Letter Ballot version
As reviewed in Jan 2023 WG-06 meeting.
</commit_message>
<xml_diff>
--- a/dictionaries/Private_Tag_Model_PC_v1.xlsx
+++ b/dictionaries/Private_Tag_Model_PC_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\abertrand\image-management\image-management\pa_dicom\PA_Private_Attr_Examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abertrand\Documents\GitHub\pa-dicom-wg34-supp229\dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE338B5-A739-4798-95BE-C0E5E94E412B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0186BB48-3A81-4D32-8B77-9F8303FB87B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="360" windowWidth="22182" windowHeight="12084" activeTab="2" xr2:uid="{C573F74A-E42E-400C-AF74-9BBE08D5972A}"/>
+    <workbookView xWindow="1404" yWindow="366" windowWidth="22182" windowHeight="12084" activeTab="3" xr2:uid="{C573F74A-E42E-400C-AF74-9BBE08D5972A}"/>
   </bookViews>
   <sheets>
     <sheet name="New Attributes" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="199">
   <si>
     <t>Tag</t>
   </si>
@@ -251,12 +251,6 @@
     <t>(gggg,ee93)</t>
   </si>
   <si>
-    <t>PA Dimension Index ID</t>
-  </si>
-  <si>
-    <t>PADimensionIndexID</t>
-  </si>
-  <si>
     <t>(gggg,a001)</t>
   </si>
   <si>
@@ -630,6 +624,18 @@
   </si>
   <si>
     <t>PhotoacousticImageStorage, temporary value of 1.2.840.10008.5.1.2.3.45</t>
+  </si>
+  <si>
+    <t>PA Reconstruction Index</t>
+  </si>
+  <si>
+    <t>PAReconstructionIndex</t>
+  </si>
+  <si>
+    <t>XXXXX5</t>
+  </si>
+  <si>
+    <t>Interstitial illumination</t>
   </si>
 </sst>
 </file>
@@ -1014,7 +1020,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1025,7 +1031,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1058,16 +1064,16 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1087,7 +1093,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G2" s="5">
         <v>0</v>
@@ -1114,7 +1120,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G3" s="5">
         <v>1</v>
@@ -1123,7 +1129,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1143,7 +1149,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G4" s="5">
         <v>1</v>
@@ -1152,7 +1158,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1172,7 +1178,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G5" s="5">
         <v>1</v>
@@ -1181,7 +1187,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1201,7 +1207,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G6" s="5">
         <v>0</v>
@@ -1228,7 +1234,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G7" s="5">
         <v>1</v>
@@ -1255,7 +1261,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G8" s="5">
         <v>0</v>
@@ -1282,7 +1288,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G9" s="5">
         <v>0</v>
@@ -1291,7 +1297,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1311,7 +1317,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G10" s="5">
         <v>0</v>
@@ -1338,7 +1344,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G11" s="5">
         <v>0</v>
@@ -1347,7 +1353,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1367,7 +1373,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G12" s="5">
         <v>0</v>
@@ -1394,7 +1400,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G13" s="5">
         <v>0</v>
@@ -1415,13 +1421,13 @@
         <v>46</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="E14" s="5">
         <v>1</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G14" s="5">
         <v>1</v>
@@ -1442,13 +1448,13 @@
         <v>50</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="E15" s="5">
         <v>1</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G15" s="5">
         <v>1</v>
@@ -1469,13 +1475,13 @@
         <v>53</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="E16" s="5">
         <v>1</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G16" s="5">
         <v>1</v>
@@ -1496,13 +1502,13 @@
         <v>56</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="E17" s="5">
         <v>1</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G17" s="5">
         <v>1</v>
@@ -1529,7 +1535,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G18" s="5">
         <v>0</v>
@@ -1538,7 +1544,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -1558,7 +1564,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G19" s="5">
         <v>0</v>
@@ -1567,7 +1573,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1587,7 +1593,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G20" s="5">
         <v>1</v>
@@ -1614,7 +1620,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G21" s="11">
         <v>1</v>
@@ -1623,7 +1629,7 @@
         <v>0</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1631,19 +1637,19 @@
         <v>69</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>70</v>
+        <v>195</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>71</v>
+        <v>196</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="E22" s="5">
         <v>1</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G22" s="5">
         <v>0</v>
@@ -1655,13 +1661,13 @@
     </row>
     <row r="23" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>72</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>74</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>8</v>
@@ -1670,7 +1676,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G23" s="11">
         <v>0</v>
@@ -1679,7 +1685,7 @@
         <v>1</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1690,10 +1696,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A19B90A7-2650-41F7-95D9-103DA39D2BF4}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1707,27 +1713,27 @@
   <sheetData>
     <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="D1" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="D2" s="8">
         <v>103401</v>
@@ -1735,13 +1741,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D3" s="8">
         <v>103402</v>
@@ -1749,13 +1755,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D4" s="8">
         <v>103403</v>
@@ -1763,127 +1769,141 @@
     </row>
     <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D5" s="8">
         <v>103404</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>138</v>
+        <v>197</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>139</v>
+        <v>198</v>
       </c>
       <c r="D6" s="8">
-        <v>103413</v>
+        <v>103405</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D7" s="8">
-        <v>103414</v>
+        <v>103413</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D8" s="8">
-        <v>103415</v>
+        <v>103414</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D9" s="8">
-        <v>103416</v>
+        <v>103415</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D10" s="8">
-        <v>103417</v>
+        <v>103416</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D11" s="8">
+        <v>103417</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" s="8">
         <v>103418</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="D12" s="8">
-        <v>103420</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D13" s="8">
+        <v>103420</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D14" s="8">
         <v>103421</v>
       </c>
     </row>
@@ -1897,7 +1917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DEB07A-7DBC-4D12-B5F3-33B25DFCC6A9}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -1918,21 +1938,21 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C2" s="5">
         <v>0</v>
@@ -1944,10 +1964,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C3" s="5">
         <v>0</v>
@@ -1959,10 +1979,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C4" s="5">
         <v>0</v>
@@ -1974,10 +1994,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C5" s="5">
         <v>0</v>
@@ -1989,10 +2009,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C6" s="5">
         <v>0</v>
@@ -2004,10 +2024,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C7" s="5">
         <v>0</v>
@@ -2019,10 +2039,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C8" s="11">
         <v>0</v>
@@ -2031,15 +2051,15 @@
         <v>0</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C9" s="11">
         <v>1</v>
@@ -2051,27 +2071,27 @@
     </row>
     <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B10" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10" s="11">
+        <v>1</v>
+      </c>
+      <c r="D10" s="11">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>106</v>
-      </c>
-      <c r="C10" s="11">
-        <v>1</v>
-      </c>
-      <c r="D10" s="11">
-        <v>0</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C11" s="11">
         <v>1</v>
@@ -2083,44 +2103,44 @@
     </row>
     <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="C12" s="5">
-        <v>0</v>
-      </c>
-      <c r="D12" s="5">
-        <v>0</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="C13" s="5">
-        <v>0</v>
-      </c>
-      <c r="D13" s="5">
-        <v>0</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C14" s="11">
         <v>1</v>
@@ -2129,15 +2149,15 @@
         <v>1</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C15" s="11">
         <v>1</v>
@@ -2149,10 +2169,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C16" s="11">
         <v>1</v>
@@ -2164,19 +2184,19 @@
     </row>
     <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="C17" s="11">
+        <v>0</v>
+      </c>
+      <c r="D17" s="11">
+        <v>0</v>
+      </c>
+      <c r="E17" s="9" t="s">
         <v>194</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="C17" s="11">
-        <v>0</v>
-      </c>
-      <c r="D17" s="11">
-        <v>0</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -2189,8 +2209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A83646B-3BAA-4FD4-957A-54A2BE427B35}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2203,7 +2223,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
@@ -2215,12 +2235,12 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -2232,12 +2252,12 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -2249,12 +2269,12 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -2266,12 +2286,12 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -2283,12 +2303,12 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -2300,12 +2320,12 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
@@ -2317,12 +2337,12 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -2334,12 +2354,12 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
@@ -2351,12 +2371,12 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B10" t="s">
         <v>31</v>
@@ -2368,29 +2388,29 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>196</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
@@ -2402,15 +2422,15 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
         <v>56</v>
@@ -2419,15 +2439,15 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
         <v>53</v>
@@ -2436,15 +2456,15 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
         <v>50</v>
@@ -2453,15 +2473,15 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
         <v>46</v>
@@ -2470,12 +2490,12 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B17" t="s">
         <v>31</v>
@@ -2487,12 +2507,12 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
@@ -2504,12 +2524,12 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B19" t="s">
         <v>12</v>
@@ -2521,12 +2541,12 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B20" t="s">
         <v>12</v>
@@ -2538,12 +2558,12 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B21" t="s">
         <v>12</v>
@@ -2555,24 +2575,24 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>